<commit_message>
updated lab 4 rubric, new lab 7 rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab04-Authorization/Lab4Rubric-Authorization.xlsx
+++ b/Labs/Lab04-Authorization/Lab4Rubric-Authorization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS296N-CourseMaterials\Labs\Lab04-Authorization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC4B0B1-05C9-4316-AEBA-2CCB645EFCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CBC827-79CC-4B8E-AC78-907D1C2A90DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33792" yWindow="4560" windowWidth="11688" windowHeight="10992" activeTab="1" xr2:uid="{30F55907-EC47-624F-8636-FE6181D07E02}"/>
+    <workbookView xWindow="33096" yWindow="5544" windowWidth="11688" windowHeight="10992" activeTab="1" xr2:uid="{30F55907-EC47-624F-8636-FE6181D07E02}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Possible</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>`</t>
+  </si>
+  <si>
+    <t>Authorization</t>
   </si>
 </sst>
 </file>
@@ -633,7 +636,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -663,7 +666,7 @@
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>